<commit_message>
Add random (Gauss with some outliers) activity duration
</commit_message>
<xml_diff>
--- a/input.sample.xlsx
+++ b/input.sample.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abos\Documents\Python\generate-process-mining-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC549AAE-4E00-48D9-9166-9D446CC5F226}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2283DD1-47FF-4137-803E-7EF6A9FEE598}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{D7EB7520-79AA-48AA-A273-C669DE671554}"/>
   </bookViews>
   <sheets>
-    <sheet name="activities" sheetId="1" r:id="rId1"/>
+    <sheet name="activity" sheetId="1" r:id="rId1"/>
     <sheet name="process_flow" sheetId="2" r:id="rId2"/>
-    <sheet name="case_properties" sheetId="3" r:id="rId3"/>
-    <sheet name="activity_properties" sheetId="4" r:id="rId4"/>
+    <sheet name="case_property" sheetId="3" r:id="rId3"/>
+    <sheet name="activity_property" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,23 +33,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
   <si>
     <t>duration</t>
   </si>
   <si>
-    <t>duration_stdev</t>
-  </si>
-  <si>
     <t>probability</t>
   </si>
   <si>
-    <t>Afdeling 1</t>
-  </si>
-  <si>
-    <t>Afdeling 2</t>
-  </si>
-  <si>
     <t>START</t>
   </si>
   <si>
@@ -83,10 +74,34 @@
     <t>next_activity_id</t>
   </si>
   <si>
-    <t>Afdeling</t>
-  </si>
-  <si>
     <t>Medewerker</t>
+  </si>
+  <si>
+    <t>Vestiging</t>
+  </si>
+  <si>
+    <t>Vestiging 1</t>
+  </si>
+  <si>
+    <t>Vestiging 2</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>outliers</t>
   </si>
 </sst>
 </file>
@@ -119,7 +134,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -471,7 +486,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66B00464-A0A5-411E-8E7D-92E8B599BA94}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -480,16 +497,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -497,26 +514,26 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2">
         <v>0</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="2" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C3" s="2">
         <v>0</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="2" t="b">
         <v>0</v>
       </c>
     </row>
@@ -530,8 +547,8 @@
       <c r="C4">
         <v>10</v>
       </c>
-      <c r="D4">
-        <v>1</v>
+      <c r="D4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -544,7 +561,7 @@
       <c r="C5">
         <v>10</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="b">
         <v>1</v>
       </c>
     </row>
@@ -556,10 +573,10 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>10</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="D6" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -572,8 +589,8 @@
       <c r="C7">
         <v>10</v>
       </c>
-      <c r="D7">
-        <v>1</v>
+      <c r="D7" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -586,7 +603,7 @@
       <c r="C8">
         <v>10</v>
       </c>
-      <c r="D8">
+      <c r="D8" t="b">
         <v>1</v>
       </c>
     </row>
@@ -598,10 +615,10 @@
         <v>6</v>
       </c>
       <c r="C9">
-        <v>10</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
+        <v>20</v>
+      </c>
+      <c r="D9" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -612,9 +629,9 @@
         <v>7</v>
       </c>
       <c r="C10">
-        <v>10</v>
-      </c>
-      <c r="D10">
+        <v>30</v>
+      </c>
+      <c r="D10" t="b">
         <v>1</v>
       </c>
     </row>
@@ -626,10 +643,10 @@
         <v>8</v>
       </c>
       <c r="C11">
-        <v>10</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
+        <v>40</v>
+      </c>
+      <c r="D11" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -640,10 +657,10 @@
         <v>9</v>
       </c>
       <c r="C12">
-        <v>10</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
+        <v>50</v>
+      </c>
+      <c r="D12" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -656,7 +673,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{653D2C56-A768-4E57-8084-FB12559EA713}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -665,13 +684,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -778,7 +797,7 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -811,7 +830,7 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -829,9 +848,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7293AFC2-F934-4038-BF39-965256578273}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -840,35 +861,79 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C2">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
       <c r="C3">
-        <v>0.5</v>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7">
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>
@@ -880,7 +945,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CE1B20-46E6-4980-A8AF-9F6BC4A06476}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -889,16 +956,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -906,10 +973,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D2">
         <v>0.4</v>
@@ -920,10 +987,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>0.5</v>
@@ -934,10 +1001,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D4">
         <v>0.1</v>

</xml_diff>